<commit_message>
Main application now implements queries modules
</commit_message>
<xml_diff>
--- a/haber.xlsx
+++ b/haber.xlsx
@@ -5814,11 +5814,11 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>592052</v>
+        <v>415948</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>MNG Mike</t>
+          <t>Yoshi</t>
         </is>
       </c>
     </row>
@@ -5848,11 +5848,11 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>415948</v>
+        <v>592052</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Yoshi</t>
+          <t>MNG Mike</t>
         </is>
       </c>
     </row>
@@ -5950,11 +5950,11 @@
         <v>9</v>
       </c>
       <c r="G18" t="n">
-        <v>592481</v>
+        <v>281841</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Riggs</t>
+          <t>rickbb</t>
         </is>
       </c>
     </row>
@@ -5984,11 +5984,11 @@
         <v>9</v>
       </c>
       <c r="G19" t="n">
-        <v>281841</v>
+        <v>592481</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>rickbb</t>
+          <t>Riggs</t>
         </is>
       </c>
     </row>
@@ -6012,15 +6012,17 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F20" t="n">
-        <v>9</v>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G20" t="n">
-        <v>225416</v>
+        <v>340348</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Wobble2King</t>
+          <t>Tury</t>
         </is>
       </c>
     </row>
@@ -6078,17 +6080,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="F22" t="n">
+        <v>9</v>
       </c>
       <c r="G22" t="n">
-        <v>587990</v>
+        <v>225416</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>TEC</t>
+          <t>Wobble2King</t>
         </is>
       </c>
     </row>
@@ -6102,27 +6102,23 @@
       <c r="C23" t="n">
         <v>9</v>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D23" t="n">
+        <v>9</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="F23" t="n">
+        <v>9</v>
       </c>
       <c r="G23" t="n">
-        <v>179962</v>
+        <v>246986</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Fran</t>
+          <t>Werito</t>
         </is>
       </c>
     </row>
@@ -6136,23 +6132,27 @@
       <c r="C24" t="n">
         <v>9</v>
       </c>
-      <c r="D24" t="n">
-        <v>9</v>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F24" t="n">
-        <v>9</v>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G24" t="n">
-        <v>246986</v>
+        <v>179962</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Werito</t>
+          <t>Fran</t>
         </is>
       </c>
     </row>
@@ -6182,11 +6182,11 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>340348</v>
+        <v>587990</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Tury</t>
+          <t>TEC</t>
         </is>
       </c>
     </row>
@@ -6394,21 +6394,27 @@
       <c r="C32" t="n">
         <v>13</v>
       </c>
-      <c r="D32" t="n">
-        <v>13</v>
-      </c>
-      <c r="E32" t="n">
-        <v>9</v>
-      </c>
-      <c r="F32" t="n">
-        <v>17</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G32" t="n">
-        <v>466335</v>
+        <v>756906</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>ViviS</t>
+          <t>Rojo</t>
         </is>
       </c>
     </row>
@@ -6422,27 +6428,21 @@
       <c r="C33" t="n">
         <v>13</v>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D33" t="n">
+        <v>13</v>
+      </c>
+      <c r="E33" t="n">
+        <v>9</v>
+      </c>
+      <c r="F33" t="n">
+        <v>17</v>
       </c>
       <c r="G33" t="n">
-        <v>1030049</v>
+        <v>466335</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Carreto</t>
+          <t>ViviS</t>
         </is>
       </c>
     </row>
@@ -6506,11 +6506,11 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>756906</v>
+        <v>1030049</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Rojo</t>
+          <t>Carreto</t>
         </is>
       </c>
     </row>
@@ -6529,18 +6529,20 @@
       <c r="D36" t="n">
         <v>17</v>
       </c>
-      <c r="E36" t="n">
-        <v>11</v>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F36" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G36" t="n">
-        <v>466863</v>
+        <v>749414</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Fabinni</t>
+          <t>Saru</t>
         </is>
       </c>
     </row>
@@ -6559,20 +6561,18 @@
       <c r="D37" t="n">
         <v>17</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="E37" t="n">
+        <v>11</v>
       </c>
       <c r="F37" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G37" t="n">
-        <v>749414</v>
+        <v>466863</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Saru</t>
+          <t>Fabinni</t>
         </is>
       </c>
     </row>
@@ -6602,11 +6602,11 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>1030453</v>
+        <v>144909</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>DOOM</t>
+          <t>Navson</t>
         </is>
       </c>
     </row>
@@ -6630,17 +6630,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="F39" t="n">
+        <v>17</v>
       </c>
       <c r="G39" t="n">
-        <v>62728</v>
+        <v>126392</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Marcopolo</t>
+          <t>Helsxan</t>
         </is>
       </c>
     </row>
@@ -6664,15 +6662,17 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F40" t="n">
-        <v>17</v>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G40" t="n">
-        <v>126392</v>
+        <v>62728</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Helsxan</t>
+          <t>Marcopolo</t>
         </is>
       </c>
     </row>
@@ -6702,11 +6702,11 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>144909</v>
+        <v>1030453</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Navson</t>
+          <t>DOOM</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Trim code, doesn't affect functionality
</commit_message>
<xml_diff>
--- a/haber.xlsx
+++ b/haber.xlsx
@@ -5407,37 +5407,37 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>avg_placing</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>border-league-round-3-melee-1-0</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>border-league-round-3-melee-2-0</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>border-league-round-3-melee-3-0</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>border-league-round-3-melee-4-0</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
         </is>
       </c>
     </row>
@@ -5449,392 +5449,392 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>38255</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bimbo</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="n">
-        <v>38255</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Bimbo</t>
-        </is>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B4" t="n">
+        <v>132537</v>
+      </c>
+      <c r="C4" t="n">
         <v>1.5</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Far!</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>132537</v>
+        <v>1</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Far!</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
+        <v>128256</v>
+      </c>
+      <c r="C5" t="n">
         <v>2.666666666666667</v>
       </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Guzy</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
         <v>4</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" t="n">
-        <v>128256</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Guzy</t>
-        </is>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>62626</v>
       </c>
       <c r="C6" t="n">
         <v>3</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Cuak</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>62626</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Cuak</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B7" t="n">
+        <v>131242</v>
+      </c>
+      <c r="C7" t="n">
         <v>3</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Hiro</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
         <v>3</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>131242</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Hiro</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="n">
+        <v>135088</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PanterA</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" t="n">
         <v>5</v>
       </c>
-      <c r="B8" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" t="n">
-        <v>5</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
         <v>3</v>
-      </c>
-      <c r="G8" t="n">
-        <v>135088</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>PanterA</t>
-        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B9" t="n">
+        <v>128266</v>
+      </c>
+      <c r="C9" t="n">
         <v>4.333333333333333</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F9" t="n">
         <v>5</v>
       </c>
       <c r="G9" t="n">
-        <v>128266</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Mike</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
+        <v>267972</v>
+      </c>
+      <c r="C10" t="n">
         <v>4.5</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
+          <t>Serch</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
         <v>4</v>
       </c>
-      <c r="F10" t="n">
+      <c r="H10" t="n">
         <v>5</v>
-      </c>
-      <c r="G10" t="n">
-        <v>267972</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Serch</t>
-        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>266941</v>
       </c>
       <c r="C11" t="n">
         <v>5</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Juanito</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>5</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G11" t="n">
-        <v>266941</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Juanito</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B12" t="n">
+        <v>35258</v>
+      </c>
+      <c r="C12" t="n">
         <v>5.25</v>
       </c>
-      <c r="C12" t="n">
-        <v>5</v>
-      </c>
-      <c r="D12" t="n">
-        <v>7</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Fist Mexico</t>
+        </is>
       </c>
       <c r="E12" t="n">
         <v>5</v>
       </c>
       <c r="F12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5</v>
+      </c>
+      <c r="H12" t="n">
         <v>4</v>
-      </c>
-      <c r="G12" t="n">
-        <v>35258</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Fist Mexico</t>
-        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B13" t="n">
+        <v>326671</v>
+      </c>
+      <c r="C13" t="n">
         <v>6</v>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Cheezburger</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
         <v>7</v>
       </c>
-      <c r="E13" t="n">
+      <c r="G13" t="n">
         <v>5</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>326671</v>
-      </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Cheezburger</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B14" t="n">
-        <v>7</v>
+        <v>592052</v>
       </c>
       <c r="C14" t="n">
         <v>7</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>MNG Mike</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>7</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G14" t="n">
-        <v>415948</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Yoshi</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B15" t="n">
-        <v>7</v>
+        <v>727335</v>
       </c>
       <c r="C15" t="n">
         <v>7</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ruby</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -5847,98 +5847,96 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G15" t="n">
-        <v>592052</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>MNG Mike</t>
-        </is>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B16" t="n">
+        <v>1133006</v>
+      </c>
+      <c r="C16" t="n">
         <v>7</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
+          <t>Yo</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
         <v>7</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
-        <v>1133006</v>
-      </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Yo</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B17" t="n">
+        <v>415948</v>
+      </c>
+      <c r="C17" t="n">
         <v>7</v>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
+          <t>Yoshi</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>7</v>
       </c>
-      <c r="G17" t="n">
-        <v>727335</v>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Ruby</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B18" t="n">
+        <v>281841</v>
+      </c>
+      <c r="C18" t="n">
         <v>9</v>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>rickbb</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -5946,33 +5944,33 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F18" t="n">
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
         <v>9</v>
-      </c>
-      <c r="G18" t="n">
-        <v>281841</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>rickbb</t>
-        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B19" t="n">
+        <v>592481</v>
+      </c>
+      <c r="C19" t="n">
         <v>9</v>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Riggs</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -5980,100 +5978,102 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F19" t="n">
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
         <v>9</v>
-      </c>
-      <c r="G19" t="n">
-        <v>592481</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Riggs</t>
-        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B20" t="n">
+        <v>416631</v>
+      </c>
+      <c r="C20" t="n">
         <v>9</v>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Monsh</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
         <v>9</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
-        <v>340348</v>
-      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Tury</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B21" t="n">
+        <v>340348</v>
+      </c>
+      <c r="C21" t="n">
         <v>9</v>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
+          <t>Tury</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
         <v>9</v>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
-        <v>416631</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Monsh</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B22" t="n">
+        <v>225416</v>
+      </c>
+      <c r="C22" t="n">
         <v>9</v>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>9</v>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Wobble2King</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -6083,27 +6083,29 @@
       <c r="F22" t="n">
         <v>9</v>
       </c>
-      <c r="G22" t="n">
-        <v>225416</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Wobble2King</t>
-        </is>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>9</v>
+        <v>587990</v>
       </c>
       <c r="C23" t="n">
         <v>9</v>
       </c>
-      <c r="D23" t="n">
-        <v>9</v>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>TEC</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -6113,290 +6115,288 @@
       <c r="F23" t="n">
         <v>9</v>
       </c>
-      <c r="G23" t="n">
-        <v>246986</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Werito</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B24" t="n">
-        <v>9</v>
+        <v>179962</v>
       </c>
       <c r="C24" t="n">
         <v>9</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Fran</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>9</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G24" t="n">
-        <v>179962</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Fran</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B25" t="n">
+        <v>246986</v>
+      </c>
+      <c r="C25" t="n">
         <v>9</v>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Werito</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
         <v>9</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
-        <v>587990</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>TEC</t>
-        </is>
+      <c r="F25" t="n">
+        <v>9</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B26" t="n">
+        <v>159127</v>
+      </c>
+      <c r="C26" t="n">
         <v>10</v>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Spon</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
         <v>13</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
         <v>7</v>
-      </c>
-      <c r="G26" t="n">
-        <v>159127</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Spon</t>
-        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B27" t="n">
+        <v>266926</v>
+      </c>
+      <c r="C27" t="n">
         <v>11</v>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Aaronman</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
         <v>9</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
         <v>13</v>
-      </c>
-      <c r="G27" t="n">
-        <v>266926</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Aaronman</t>
-        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B28" t="n">
+        <v>547528</v>
+      </c>
+      <c r="C28" t="n">
         <v>11.5</v>
       </c>
-      <c r="C28" t="n">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
         <v>9</v>
       </c>
-      <c r="D28" t="n">
+      <c r="F28" t="n">
         <v>17</v>
       </c>
-      <c r="E28" t="n">
+      <c r="G28" t="n">
         <v>7</v>
       </c>
-      <c r="F28" t="n">
+      <c r="H28" t="n">
         <v>13</v>
-      </c>
-      <c r="G28" t="n">
-        <v>547528</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Min</t>
-        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B29" t="n">
+        <v>756906</v>
+      </c>
+      <c r="C29" t="n">
         <v>13</v>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
+          <t>Rojo</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
         <v>13</v>
       </c>
-      <c r="G29" t="n">
-        <v>1193165</v>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Andygibb</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B30" t="n">
+        <v>1030049</v>
+      </c>
+      <c r="C30" t="n">
         <v>13</v>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Carreto</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
         <v>13</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G30" t="n">
-        <v>274638</v>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>pepino de mar</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B31" t="n">
+        <v>176667</v>
+      </c>
+      <c r="C31" t="n">
         <v>13</v>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Dodo</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
         <v>13</v>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G31" t="n">
-        <v>176667</v>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Dodo</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B32" t="n">
-        <v>13</v>
+        <v>274638</v>
       </c>
       <c r="C32" t="n">
         <v>13</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>pepino de mar</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -6404,225 +6404,225 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
-        <v>756906</v>
+      <c r="F32" t="n">
+        <v>13</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Rojo</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B33" t="n">
-        <v>13</v>
+        <v>1193165</v>
       </c>
       <c r="C33" t="n">
         <v>13</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Andygibb</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
         <v>13</v>
-      </c>
-      <c r="E33" t="n">
-        <v>9</v>
-      </c>
-      <c r="F33" t="n">
-        <v>17</v>
-      </c>
-      <c r="G33" t="n">
-        <v>466335</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>ViviS</t>
-        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B34" t="n">
-        <v>13</v>
+        <v>466335</v>
       </c>
       <c r="C34" t="n">
         <v>13</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>ViviS</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>13</v>
+      </c>
+      <c r="F34" t="n">
+        <v>13</v>
       </c>
       <c r="G34" t="n">
-        <v>137183</v>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Trujillo</t>
-        </is>
+        <v>9</v>
+      </c>
+      <c r="H34" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B35" t="n">
-        <v>13</v>
+        <v>137183</v>
       </c>
       <c r="C35" t="n">
         <v>13</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Trujillo</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>13</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G35" t="n">
-        <v>1030049</v>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Carreto</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B36" t="n">
+        <v>749414</v>
+      </c>
+      <c r="C36" t="n">
         <v>15</v>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Saru</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
         <v>17</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
         <v>13</v>
-      </c>
-      <c r="G36" t="n">
-        <v>749414</v>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Saru</t>
-        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B37" t="n">
+        <v>466863</v>
+      </c>
+      <c r="C37" t="n">
         <v>15</v>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>17</v>
-      </c>
-      <c r="E37" t="n">
-        <v>11</v>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Fabinni</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F37" t="n">
         <v>17</v>
       </c>
       <c r="G37" t="n">
-        <v>466863</v>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Fabinni</t>
-        </is>
+        <v>11</v>
+      </c>
+      <c r="H37" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B38" t="n">
+        <v>62728</v>
+      </c>
+      <c r="C38" t="n">
         <v>17</v>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Marcopolo</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
         <v>17</v>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="F38" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G38" t="n">
-        <v>144909</v>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Navson</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B39" t="n">
-        <v>17</v>
+        <v>1071485</v>
       </c>
       <c r="C39" t="n">
         <v>17</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Mr.L</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -6633,28 +6633,30 @@
       <c r="F39" t="n">
         <v>17</v>
       </c>
-      <c r="G39" t="n">
-        <v>126392</v>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Helsxan</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B40" t="n">
-        <v>17</v>
+        <v>1030453</v>
       </c>
       <c r="C40" t="n">
         <v>17</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>DOOM</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -6662,85 +6664,83 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G40" t="n">
-        <v>62728</v>
+      <c r="F40" t="n">
+        <v>17</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Marcopolo</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B41" t="n">
+        <v>126392</v>
+      </c>
+      <c r="C41" t="n">
         <v>17</v>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Helsxan</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
         <v>17</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="F41" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G41" t="n">
-        <v>1030453</v>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>DOOM</t>
-        </is>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B42" t="n">
+        <v>144909</v>
+      </c>
+      <c r="C42" t="n">
         <v>17</v>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Navson</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
         <v>17</v>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G42" t="n">
-        <v>1071485</v>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Mr.L</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -6749,16 +6749,14 @@
         <v>40</v>
       </c>
       <c r="B43" t="n">
+        <v>675175</v>
+      </c>
+      <c r="C43" t="n">
         <v>17</v>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Mirage</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -6766,16 +6764,18 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F43" t="n">
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
         <v>17</v>
-      </c>
-      <c r="G43" t="n">
-        <v>675175</v>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Mirage</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>